<commit_message>
Added design doc, task sheet, and user stories
</commit_message>
<xml_diff>
--- a/Attendance Project Group 2 Task Sheet.xlsx
+++ b/Attendance Project Group 2 Task Sheet.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Evolution 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Evolution 2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="224">
   <si>
     <t>Task</t>
   </si>
@@ -234,41 +234,506 @@
     <t>TextUserView Class</t>
   </si>
   <si>
+    <t>Sub-Program</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">we may change the ArrayList&lt;Course&gt; from class Professor to  ArrayList&lt;Section&gt; so that section info can be stored. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Section class </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">can include Course and Int number,  String ID as arrtibutes </t>
+    </r>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
     <t>Client</t>
   </si>
   <si>
-    <t>Register Class</t>
-  </si>
-  <si>
-    <t>LoginRequest Class</t>
-  </si>
-  <si>
-    <t>Shared</t>
+    <t>Qianyi &amp; Louise</t>
+  </si>
+  <si>
+    <t>4/8-4/11</t>
+  </si>
+  <si>
+    <t>Faculty &amp; Student</t>
+  </si>
+  <si>
+    <t>logIn</t>
+  </si>
+  <si>
+    <t>TextUserController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">receive id and passwords -&gt; send to server -&gt; check whether correct on server side with database -&gt; return the result </t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>loadProfessor</t>
+  </si>
+  <si>
+    <t>successfully log in -&gt; request all required info from database and send a professor obj back</t>
+  </si>
+  <si>
+    <t>addNewCourse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">load all courses from database -&gt; add a course -&gt; check whether currently teach this course -&gt; if not add the course to this Professor obj -&gt; send the Course info to the server and store in database  </t>
+  </si>
+  <si>
+    <t>addSection</t>
+  </si>
+  <si>
+    <t>should be inside addNewCourse</t>
+  </si>
+  <si>
+    <t>select the course -&gt; select the section -&gt; send the data to server and database</t>
+  </si>
+  <si>
+    <t>takeAttendance</t>
+  </si>
+  <si>
+    <t>select the course-&gt;select the section-&gt; start new Lecture -&gt; load students from database -&gt; show students' name -&gt; take attendance -&gt; send the records to database</t>
+  </si>
+  <si>
+    <t>updateAttendance</t>
+  </si>
+  <si>
+    <t>select the course &amp; section -&gt; use course &amp; section info to get all lectures by date from database -&gt; show the lectures to users -&gt; choose the exact lecture-&gt;get the attendance -&gt; update the attendance -&gt; send back to database</t>
+  </si>
+  <si>
+    <t>takeAttendanceFromPreviousDay</t>
+  </si>
+  <si>
+    <t>Not sure whether still need it if using updateAttendance</t>
   </si>
   <si>
     <t>AttendanceRecord Class</t>
   </si>
   <si>
+    <t>showReportForStudent</t>
+  </si>
+  <si>
+    <t>choose course &amp; section -&gt; get all students' records by the info (need to get the participation grade on server side)</t>
+  </si>
+  <si>
     <t>AttendanceSession Class</t>
   </si>
   <si>
     <t>Server</t>
   </si>
   <si>
+    <t>Student class may also need ArrayList&lt;Section&gt;</t>
+  </si>
+  <si>
     <t>Notifier Interface</t>
   </si>
   <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>loadStudent</t>
+  </si>
+  <si>
+    <t>log in -&gt; request all required info from database and send a student obj back</t>
+  </si>
+  <si>
     <t>EmailNotifier Class</t>
   </si>
   <si>
+    <t>changeNotificationPreference</t>
+  </si>
+  <si>
+    <t>select Course -&gt; show preference -&gt; change or not -&gt; if yes send to server and update the record</t>
+  </si>
+  <si>
     <t>UserAuthentication Class</t>
+  </si>
+  <si>
+    <t>getReportSummary</t>
+  </si>
+  <si>
+    <t>select Course -&gt; get record with sectionID &amp; calculate the participation points on server side -&gt; send to client and show results</t>
+  </si>
+  <si>
+    <t>Database design</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>integration, send socket and send specific command to run each function</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Display Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>University ID</t>
+  </si>
+  <si>
+    <t>Instructor</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t>plain server</t>
+  </si>
+  <si>
+    <t>checkMatch(id,password)</t>
+  </si>
+  <si>
+    <t>check id and password through database. send -1 to client if not match, 0 faculty, 1 student</t>
+  </si>
+  <si>
+    <t>Course ID</t>
+  </si>
+  <si>
+    <t>Instructor ID</t>
+  </si>
+  <si>
+    <t>logInHandler()</t>
+  </si>
+  <si>
+    <t>send a professor obj</t>
+  </si>
+  <si>
+    <t>Lecture</t>
+  </si>
+  <si>
+    <t>Section ID</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>ClientHandler()</t>
+  </si>
+  <si>
+    <t>send a student obj</t>
+  </si>
+  <si>
+    <t>Enrollment</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>allCoursesInDatabase</t>
+  </si>
+  <si>
+    <t>send a list of Courses in Database</t>
+  </si>
+  <si>
+    <t>Attendance</t>
+  </si>
+  <si>
+    <t>Lecture ID</t>
+  </si>
+  <si>
+    <t>allSectionsofCourse</t>
+  </si>
+  <si>
+    <t>send all sections of a Course in Database</t>
+  </si>
+  <si>
+    <t>Passwords</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>let id be a faculty in SectionID</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>ChangeName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notification </t>
+  </si>
+  <si>
+    <t>student ID</t>
+  </si>
+  <si>
+    <t>On/Off</t>
+  </si>
+  <si>
+    <t>getStudents(Section ID)</t>
+  </si>
+  <si>
+    <t>send list of students back</t>
+  </si>
+  <si>
+    <t>no need to send anything?</t>
+  </si>
+  <si>
+    <t>Student getStudent(String id)</t>
+  </si>
+  <si>
+    <t>updateAttendance(LectureID,HashMap&lt;student ID,AttendanceStatus&gt;&gt;)</t>
+  </si>
+  <si>
+    <t>set the info to database</t>
+  </si>
+  <si>
+    <t>sendEmail(Student ID,Lecture ID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get the courseID by lecture ID and check whether the Student ID's preference is on. If on, send the AttendaceRecord by Lecture ID </t>
+  </si>
+  <si>
+    <t>AttendanceRecord getStudentStatus(Student student, Lecture lecture)</t>
+  </si>
+  <si>
+    <t>getLectures(Section ID)</t>
+  </si>
+  <si>
+    <t>send a list of Lecture to client</t>
+  </si>
+  <si>
+    <t>boolean checkPassword(String password, String ID)</t>
+  </si>
+  <si>
+    <t>getAttendanceRecordsByLecture(Lecture ID)</t>
+  </si>
+  <si>
+    <t>send a list of records by lecture ID</t>
+  </si>
+  <si>
+    <t>updateAttendance(Lecture ID,Student ID,AttendanceStatus)</t>
+  </si>
+  <si>
+    <t>change the attendanceStatus of student id by selecting exact lecture ID</t>
+  </si>
+  <si>
+    <t>getStudentsRecords(Section ID)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">get and send back a HashMap&lt;Student, AttendanceRecordSummary&gt;. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>AttendaceRecordSummay</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> can be a new class includes arraylist of AttendanceRecord from one course and the score of the student</t>
+    </r>
+  </si>
+  <si>
+    <t>calculateScore(ArrayList&lt;AttendanceStatus&gt;)</t>
+  </si>
+  <si>
+    <t>get a score for attendance of a student in one course</t>
+  </si>
+  <si>
+    <t>updatePreference(Course ID,Student ID, boolean on)</t>
+  </si>
+  <si>
+    <t>change to turn on/off the notification by boolean on</t>
+  </si>
+  <si>
+    <t>getAttendanceRecordSummaryForOne(Section ID,Student ID)</t>
+  </si>
+  <si>
+    <t>getInfoFromDatabase(...)</t>
+  </si>
+  <si>
+    <t>get the CourseID, SectionID by Lecture ID</t>
+  </si>
+  <si>
+    <t>IntegrationAttendanceRecordInfo(...)</t>
+  </si>
+  <si>
+    <t>one AttendanceRecord should include course name, student ID, Date,Status</t>
+  </si>
+  <si>
+    <t>DAOFunctions</t>
+  </si>
+  <si>
+    <t>receive the socket, and choose different functions to run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CourseManagement </t>
+  </si>
+  <si>
+    <t>addCourse(courseName,int sections)</t>
+  </si>
+  <si>
+    <t>assign a course ID for this course, create sections for this course in database</t>
+  </si>
+  <si>
+    <t>getSection(courseID)</t>
+  </si>
+  <si>
+    <t>get the number of sections in a Course</t>
+  </si>
+  <si>
+    <t>addSection(courseID)</t>
+  </si>
+  <si>
+    <t>add a new Section</t>
+  </si>
+  <si>
+    <t>enrollStudents(SectionID)</t>
+  </si>
+  <si>
+    <t>load students with below methods and put them to database</t>
+  </si>
+  <si>
+    <t>loadStudentsByCSV</t>
+  </si>
+  <si>
+    <t>return a list of students</t>
+  </si>
+  <si>
+    <t>loadStudentManually</t>
+  </si>
+  <si>
+    <t>return a student</t>
+  </si>
+  <si>
+    <t>removeSection(SectionID)</t>
+  </si>
+  <si>
+    <t>delete everything related with this Section</t>
+  </si>
+  <si>
+    <t>removeCourse(CourseID)</t>
+  </si>
+  <si>
+    <t>delete everything related with this Cours</t>
+  </si>
+  <si>
+    <t>updateCourseName(CourseID)</t>
+  </si>
+  <si>
+    <t>dropStudent(ID,SectionID)</t>
+  </si>
+  <si>
+    <t>CourseManagementTextView</t>
+  </si>
+  <si>
+    <t>What will update Class/Section DO???</t>
+  </si>
+  <si>
+    <t>CourseManagementApp</t>
+  </si>
+  <si>
+    <t>UserRegistration</t>
+  </si>
+  <si>
+    <t>4/5-4/11</t>
+  </si>
+  <si>
+    <t>addStudent(id, password)</t>
+  </si>
+  <si>
+    <t>register user</t>
+  </si>
+  <si>
+    <t>addProfessor(id,password)</t>
+  </si>
+  <si>
+    <t>removeUser(id)</t>
+  </si>
+  <si>
+    <t>delete user</t>
+  </si>
+  <si>
+    <t>updateUser(id,password)</t>
+  </si>
+  <si>
+    <t>change passwords</t>
+  </si>
+  <si>
+    <t>updatePasswords(id,newPassword)</t>
+  </si>
+  <si>
+    <t>UserRegistrationTextView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">similar to E1 TextView </t>
+  </si>
+  <si>
+    <t>UserRegistrationApp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -306,8 +771,21 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +808,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
         <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -383,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -444,7 +928,49 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1934,169 +2460,838 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="15.0"/>
     <col customWidth="1" min="2" max="2" width="23.0"/>
+    <col customWidth="1" min="7" max="7" width="14.63"/>
+    <col customWidth="1" min="8" max="11" width="16.5"/>
+    <col customWidth="1" min="12" max="12" width="36.25"/>
+    <col customWidth="1" min="13" max="13" width="28.25"/>
+    <col customWidth="1" min="14" max="14" width="168.0"/>
+    <col customWidth="1" min="15" max="15" width="142.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
+      <c r="H1" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
-        <v>73</v>
+      <c r="A2" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>69</v>
       </c>
+      <c r="H2" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="17" t="s">
-        <v>74</v>
+        <v>89</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="17" t="s">
-        <v>75</v>
+      <c r="B4" s="17"/>
+      <c r="I4" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="17"/>
+      <c r="I5" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="17" t="s">
-        <v>62</v>
+      <c r="I6" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>70</v>
+        <v>62</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>78</v>
+        <v>104</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="21" t="s">
-        <v>79</v>
-      </c>
       <c r="B10" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="17" t="s">
-        <v>80</v>
+      <c r="I11" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>81</v>
+        <v>110</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>82</v>
+        <v>114</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="20"/>
+      <c r="B14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="20"/>
+      <c r="I15" s="21" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="16">
-      <c r="B16" s="20"/>
+      <c r="A16" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="I16" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="17">
-      <c r="B17" s="20"/>
+      <c r="B17" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="18">
-      <c r="B18" s="20"/>
+      <c r="B18" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="25"/>
     </row>
     <row r="19">
-      <c r="B19" s="20"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="M19" s="25"/>
+      <c r="N19" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
     </row>
     <row r="20">
-      <c r="B20" s="20"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="I20" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="21">
-      <c r="B21" s="20"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="I21" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="N21" s="21" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="22">
-      <c r="B22" s="20"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="I22" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="N22" s="21" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="23">
-      <c r="B23" s="20"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="I23" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L23" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="N23" s="21" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="24">
-      <c r="B24" s="20"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="I24" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="25">
-      <c r="B25" s="20"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="25"/>
+      <c r="I25" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="L25" s="21"/>
+      <c r="N25" s="21"/>
     </row>
     <row r="26">
-      <c r="B26" s="20"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="I26" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="27">
-      <c r="B27" s="20"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="I27" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="28">
-      <c r="B28" s="20"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="I28" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L28" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="N28" s="21" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="29">
-      <c r="B29" s="20"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="I29" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L29" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="N29" s="21" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="30">
-      <c r="B30" s="20"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="I30" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L30" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="N30" s="21" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="31">
-      <c r="B31" s="20"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="I31" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L31" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="N31" s="21" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="32">
-      <c r="B32" s="20"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="I32" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L32" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="N32" s="21" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="33">
       <c r="B33" s="20"/>
+      <c r="I33" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L33" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="N33" s="21" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="20"/>
+      <c r="I34" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L34" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="N34" s="21" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" s="20"/>
+      <c r="I35" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L35" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="N35" s="21" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="36">
       <c r="B36" s="20"/>
+      <c r="I36" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J36" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L36" s="21" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="20"/>
+      <c r="I37" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J37" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L37" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="N37" s="21" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="38">
       <c r="B38" s="20"/>
+      <c r="I38" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L38" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="N38" s="21" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="39">
       <c r="B39" s="20"/>
     </row>
     <row r="40">
       <c r="B40" s="20"/>
+      <c r="I40" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L40" s="21" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="41">
       <c r="B41" s="20"/>
     </row>
     <row r="42">
       <c r="B42" s="20"/>
+      <c r="I42" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J42" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L42" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="N42" s="21" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" s="20"/>
@@ -2106,78 +3301,284 @@
     </row>
     <row r="45">
       <c r="B45" s="20"/>
+      <c r="H45" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L45" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="N45" s="21" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" s="20"/>
+      <c r="I46" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L46" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="N46" s="33" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="20"/>
+      <c r="I47" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L47" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="N47" s="21" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="48">
       <c r="B48" s="20"/>
+      <c r="I48" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L48" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="N48" s="21" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="49">
       <c r="B49" s="20"/>
+      <c r="I49" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L49" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="N49" s="21" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="50">
       <c r="B50" s="20"/>
+      <c r="I50" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L50" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="N50" s="21" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="51">
       <c r="B51" s="20"/>
+      <c r="I51" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L51" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="N51" s="21" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" s="20"/>
+      <c r="I52" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L52" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="N52" s="21" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="53">
       <c r="B53" s="20"/>
+      <c r="I53" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L53" s="34" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="54">
       <c r="B54" s="20"/>
+      <c r="I54" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L54" s="34" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="55">
       <c r="B55" s="20"/>
+      <c r="I55" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L55" s="34" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="56">
       <c r="B56" s="20"/>
+      <c r="I56" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L56" s="35" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="57">
       <c r="B57" s="20"/>
+      <c r="I57" s="21" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="58">
       <c r="B58" s="20"/>
+      <c r="I58" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L58" s="21" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="59">
       <c r="B59" s="20"/>
     </row>
     <row r="60">
       <c r="B60" s="20"/>
+      <c r="H60" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="I60" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="K60" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="L60" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="M60" s="21"/>
+      <c r="N60" s="21" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="61">
       <c r="B61" s="20"/>
+      <c r="I61" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J61" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L61" s="21" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="62">
       <c r="B62" s="20"/>
+      <c r="I62" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J62" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L62" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="N62" s="21" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="63">
       <c r="B63" s="20"/>
+      <c r="I63" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L63" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="N63" s="21" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="64">
       <c r="B64" s="20"/>
+      <c r="I64" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J64" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L64" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="N64" s="21"/>
     </row>
     <row r="65">
       <c r="B65" s="20"/>
+      <c r="I65" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J65" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L65" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="N65" s="21" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="66">
       <c r="B66" s="20"/>
+      <c r="I66" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L66" s="34"/>
     </row>
     <row r="67">
       <c r="B67" s="20"/>
+      <c r="I67" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L67" s="35"/>
     </row>
     <row r="68">
       <c r="B68" s="20"/>
+      <c r="I68" s="21" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="69">
       <c r="B69" s="20"/>
+      <c r="I69" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J69" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L69" s="21" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="70">
       <c r="B70" s="20"/>
@@ -4972,11 +6373,56 @@
     <row r="1000">
       <c r="B1000" s="20"/>
     </row>
+    <row r="1001">
+      <c r="B1001" s="20"/>
+    </row>
+    <row r="1002">
+      <c r="B1002" s="20"/>
+    </row>
+    <row r="1003">
+      <c r="B1003" s="20"/>
+    </row>
+    <row r="1004">
+      <c r="B1004" s="20"/>
+    </row>
+    <row r="1005">
+      <c r="B1005" s="20"/>
+    </row>
+    <row r="1006">
+      <c r="B1006" s="20"/>
+    </row>
+    <row r="1007">
+      <c r="B1007" s="20"/>
+    </row>
+    <row r="1008">
+      <c r="B1008" s="20"/>
+    </row>
+    <row r="1009">
+      <c r="B1009" s="20"/>
+    </row>
+    <row r="1010">
+      <c r="B1010" s="20"/>
+    </row>
+    <row r="1011">
+      <c r="B1011" s="20"/>
+    </row>
+    <row r="1012">
+      <c r="B1012" s="20"/>
+    </row>
+    <row r="1013">
+      <c r="B1013" s="20"/>
+    </row>
+    <row r="1014">
+      <c r="B1014" s="20"/>
+    </row>
+    <row r="1015">
+      <c r="B1015" s="20"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>